<commit_message>
Commit and push with Automation HUB process
</commit_message>
<xml_diff>
--- a/Data/Temp/Yearly-Report-2021-DE325476.xlsx
+++ b/Data/Temp/Yearly-Report-2021-DE325476.xlsx
@@ -16,10 +16,85 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <x:si>
+    <x:t>433134</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Beverages and Catering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-03-17</x:t>
+  </x:si>
+  <x:si>
+    <x:t>33348</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6669.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>40017.6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RON</x:t>
+  </x:si>
+  <x:si>
+    <x:t>360581</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-05-11</x:t>
+  </x:si>
+  <x:si>
+    <x:t>248832</x:t>
+  </x:si>
+  <x:si>
+    <x:t>49766.4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>298598</x:t>
+  </x:si>
+  <x:si>
+    <x:t>CAD</x:t>
+  </x:si>
+  <x:si>
+    <x:t>531742</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-05-26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>183694</x:t>
+  </x:si>
+  <x:si>
+    <x:t>36738.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>220433</x:t>
+  </x:si>
+  <x:si>
+    <x:t>EUR</x:t>
+  </x:si>
+  <x:si>
+    <x:t>709464</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Waste management services</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-05-19</x:t>
+  </x:si>
+  <x:si>
+    <x:t>259031</x:t>
+  </x:si>
+  <x:si>
+    <x:t>51806.2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>310837</x:t>
+  </x:si>
+  <x:si>
     <x:t>329202</x:t>
   </x:si>
   <x:si>
-    <x:t>Waste management services</x:t>
+    <x:t>2017-06-24</x:t>
   </x:si>
   <x:si>
     <x:t>137553</x:t>
@@ -31,36 +106,30 @@
     <x:t>165064</x:t>
   </x:si>
   <x:si>
-    <x:t>CAD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-06-24</x:t>
-  </x:si>
-  <x:si>
-    <x:t>433134</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Beverages and Catering</x:t>
-  </x:si>
-  <x:si>
-    <x:t>33348</x:t>
-  </x:si>
-  <x:si>
-    <x:t>6669.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>40017.6</x:t>
-  </x:si>
-  <x:si>
-    <x:t>RON</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-03-17</x:t>
+    <x:t>399663</x:t>
+  </x:si>
+  <x:si>
+    <x:t>IT Support</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2017-08-09</x:t>
+  </x:si>
+  <x:si>
+    <x:t>286554</x:t>
+  </x:si>
+  <x:si>
+    <x:t>57310.8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>343865</x:t>
   </x:si>
   <x:si>
     <x:t>824831</x:t>
   </x:si>
   <x:si>
+    <x:t>2017-09-27</x:t>
+  </x:si>
+  <x:si>
     <x:t>144846</x:t>
   </x:si>
   <x:si>
@@ -73,81 +142,15 @@
     <x:t>USD</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-09-27</x:t>
-  </x:si>
-  <x:si>
-    <x:t>360581</x:t>
-  </x:si>
-  <x:si>
-    <x:t>248832</x:t>
-  </x:si>
-  <x:si>
-    <x:t>49766.4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>298598</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-05-11</x:t>
-  </x:si>
-  <x:si>
-    <x:t>531742</x:t>
-  </x:si>
-  <x:si>
-    <x:t>183694</x:t>
-  </x:si>
-  <x:si>
-    <x:t>36738.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>220433</x:t>
-  </x:si>
-  <x:si>
-    <x:t>EUR</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-05-26</x:t>
-  </x:si>
-  <x:si>
-    <x:t>709464</x:t>
-  </x:si>
-  <x:si>
-    <x:t>259031</x:t>
-  </x:si>
-  <x:si>
-    <x:t>51806.2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>310837</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-05-19</x:t>
-  </x:si>
-  <x:si>
-    <x:t>399663</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IT Support</x:t>
-  </x:si>
-  <x:si>
-    <x:t>286554</x:t>
-  </x:si>
-  <x:si>
-    <x:t>57310.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>343865</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-08-09</x:t>
-  </x:si>
-  <x:si>
     <x:t>476181</x:t>
   </x:si>
   <x:si>
     <x:t>Concierge Services</x:t>
   </x:si>
   <x:si>
+    <x:t>2017-10-18</x:t>
+  </x:si>
+  <x:si>
     <x:t>118203</x:t>
   </x:si>
   <x:si>
@@ -157,15 +160,15 @@
     <x:t>141844</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-10-18</x:t>
-  </x:si>
-  <x:si>
     <x:t>502515</x:t>
   </x:si>
   <x:si>
     <x:t>Professional Services</x:t>
   </x:si>
   <x:si>
+    <x:t>2017-10-21</x:t>
+  </x:si>
+  <x:si>
     <x:t>57773</x:t>
   </x:si>
   <x:si>
@@ -175,12 +178,12 @@
     <x:t>69327.6</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-10-21</x:t>
-  </x:si>
-  <x:si>
     <x:t>739981</x:t>
   </x:si>
   <x:si>
+    <x:t>2017-10-10</x:t>
+  </x:si>
+  <x:si>
     <x:t>14987</x:t>
   </x:si>
   <x:si>
@@ -190,12 +193,12 @@
     <x:t>17984.4</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-10-10</x:t>
-  </x:si>
-  <x:si>
     <x:t>736621</x:t>
   </x:si>
   <x:si>
+    <x:t>2017-10-23</x:t>
+  </x:si>
+  <x:si>
     <x:t>3022</x:t>
   </x:si>
   <x:si>
@@ -205,12 +208,12 @@
     <x:t>3626.4</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-10-23</x:t>
-  </x:si>
-  <x:si>
     <x:t>326522</x:t>
   </x:si>
   <x:si>
+    <x:t>2017-12-11</x:t>
+  </x:si>
+  <x:si>
     <x:t>85056</x:t>
   </x:si>
   <x:si>
@@ -220,12 +223,12 @@
     <x:t>102067</x:t>
   </x:si>
   <x:si>
-    <x:t>2017-12-11</x:t>
-  </x:si>
-  <x:si>
     <x:t>850184</x:t>
   </x:si>
   <x:si>
+    <x:t>2017-12-04</x:t>
+  </x:si>
+  <x:si>
     <x:t>53294</x:t>
   </x:si>
   <x:si>
@@ -233,9 +236,6 @@
   </x:si>
   <x:si>
     <x:t>63952.8</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2017-12-04</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -617,140 +617,140 @@
     </x:row>
     <x:row r="2" spans="1:7">
       <x:c r="A2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>0</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>2</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>3</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>4</x:v>
       </x:c>
       <x:c r="F2" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>5</x:v>
       </x:c>
       <x:c r="G2" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:7">
       <x:c r="A3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>11</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:7">
       <x:c r="A4" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>15</x:v>
       </x:c>
       <x:c r="E4" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="F4" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="G4" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:7">
       <x:c r="A5" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>19</x:v>
       </x:c>
       <x:c r="B5" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>21</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:7">
       <x:c r="A6" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>1</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:7">
       <x:c r="A7" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
         <x:v>18</x:v>
-      </x:c>
-      <x:c r="G7" s="0" t="s">
-        <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:7">
@@ -758,19 +758,19 @@
         <x:v>36</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
+      <x:c r="D8" s="0" t="s">
         <x:v>38</x:v>
       </x:c>
-      <x:c r="D8" s="0" t="s">
+      <x:c r="E8" s="0" t="s">
         <x:v>39</x:v>
       </x:c>
-      <x:c r="E8" s="0" t="s">
+      <x:c r="F8" s="0" t="s">
         <x:v>40</x:v>
-      </x:c>
-      <x:c r="F8" s="0" t="s">
-        <x:v>29</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
         <x:v>41</x:v>
@@ -778,140 +778,140 @@
     </x:row>
     <x:row r="9" spans="1:7">
       <x:c r="A9" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>18</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>19</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:7">
       <x:c r="A10" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:7">
       <x:c r="A11" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:7">
       <x:c r="A12" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
         <x:v>1</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>58</x:v>
+        <x:v>6</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:7">
       <x:c r="A13" s="0" t="s">
-        <x:v>59</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>1</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>60</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>61</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>62</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>63</x:v>
+        <x:v>18</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:7">
       <x:c r="A14" s="0" t="s">
-        <x:v>64</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>65</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>66</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>67</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>68</x:v>
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="15" spans="1:7">
@@ -922,19 +922,19 @@
         <x:v>43</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="D15" s="0" t="s">
+        <x:v>72</x:v>
+      </x:c>
+      <x:c r="E15" s="0" t="s">
+        <x:v>73</x:v>
+      </x:c>
+      <x:c r="F15" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="G15" s="0" t="s">
         <x:v>70</x:v>
-      </x:c>
-      <x:c r="D15" s="0" t="s">
-        <x:v>71</x:v>
-      </x:c>
-      <x:c r="E15" s="0" t="s">
-        <x:v>72</x:v>
-      </x:c>
-      <x:c r="F15" s="0" t="s">
-        <x:v>5</x:v>
-      </x:c>
-      <x:c r="G15" s="0" t="s">
-        <x:v>73</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>